<commit_message>
fixed links from updating site structure
</commit_message>
<xml_diff>
--- a/week1/TimeSheets.xlsx
+++ b/week1/TimeSheets.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bhislop/Documents/school/classes/2025-6-spring/cs-4360-experience/notes/week1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bhislop/Documents/school/classes/2025-6-spring/cs-4360-experience/notes/week1/week1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08B170C1-4CD8-D745-BE7E-29695C8267CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B551DDB1-4CB3-084A-B12B-5A4F489B6E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{82D859AA-A28A-3C43-A1A9-9F175A2BEA5D}"/>
+    <workbookView xWindow="-76800" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{82D859AA-A28A-3C43-A1A9-9F175A2BEA5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,12 +77,6 @@
     <t>2 (in class)</t>
   </si>
   <si>
-    <t>https://github.com/Bphissles/cs4360-class-notes/blob/main/jan-21.md</t>
-  </si>
-  <si>
-    <t>https://github.com/Bphissles/cs4360-class-notes/blob/main/jan-23.md</t>
-  </si>
-  <si>
     <t>Better Idea of what the end of class deliverable will be</t>
   </si>
   <si>
@@ -111,13 +105,19 @@
   </si>
   <si>
     <t>Found out a lot about static site generation. Got to know some classmates, and a feel for what they want out of this class. Started to realize what I want from the class.</t>
+  </si>
+  <si>
+    <t>https://github.com/Bphissles/cs4360-class-notes/blob/main/week1/jan-21.md</t>
+  </si>
+  <si>
+    <t>https://github.com/Bphissles/cs4360-class-notes/blob/main/week1/jan-23.md</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -191,14 +191,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="14"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -389,7 +381,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -398,25 +390,31 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -446,13 +444,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -793,7 +785,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -807,22 +799,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="28" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="17"/>
     </row>
     <row r="2" spans="1:5" ht="27" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="18"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="20"/>
     </row>
     <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -839,18 +831,18 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="40" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>45678</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>15</v>
       </c>
       <c r="E4" s="4"/>
     </row>
@@ -858,88 +850,88 @@
       <c r="A5" s="5">
         <v>45680</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>16</v>
       </c>
       <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" ht="80" x14ac:dyDescent="0.2">
-      <c r="A6" s="8">
+      <c r="A6" s="7">
         <v>45682</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>20</v>
+      <c r="D6" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5" ht="80" x14ac:dyDescent="0.2">
-      <c r="A7" s="8">
+      <c r="A7" s="7">
         <v>45684</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>22</v>
+      <c r="B7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" ht="25" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="21"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="23"/>
     </row>
     <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="101" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22">
+      <c r="A10" s="12">
         <v>9.8000000000000007</v>
       </c>
-      <c r="B10" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="23">
+      <c r="B10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="13">
         <v>-2.2000000000000002</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="13">
         <v>-2.2000000000000002</v>
       </c>
-      <c r="E10" s="24" t="s">
-        <v>24</v>
+      <c r="E10" s="14" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>